<commit_message>
remove diameter from shot metadata
</commit_message>
<xml_diff>
--- a/shot_metadata.xlsx
+++ b/shot_metadata.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Shot</t>
   </si>
@@ -22,16 +22,10 @@
     <t>Shot weight</t>
   </si>
   <si>
-    <t>Shot diameter</t>
-  </si>
-  <si>
     <t>Nr</t>
   </si>
   <si>
     <t>kg</t>
-  </si>
-  <si>
-    <t>mm</t>
   </si>
 </sst>
 </file>
@@ -101,23 +95,19 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="D1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="2">
@@ -129,9 +119,7 @@
       <c r="C3" s="2">
         <v>10.5</v>
       </c>
-      <c r="D3" s="2">
-        <v>141.3</v>
-      </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="2">
@@ -143,9 +131,7 @@
       <c r="C4" s="2">
         <v>10.47</v>
       </c>
-      <c r="D4" s="2">
-        <v>141.8</v>
-      </c>
+      <c r="D4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="2">
@@ -157,9 +143,7 @@
       <c r="C5" s="2">
         <v>10.52</v>
       </c>
-      <c r="D5" s="2">
-        <v>141.8</v>
-      </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="2">
@@ -171,9 +155,7 @@
       <c r="C6" s="2">
         <v>10.47</v>
       </c>
-      <c r="D6" s="2">
-        <v>141.2</v>
-      </c>
+      <c r="D6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="2">
@@ -185,9 +167,7 @@
       <c r="C7" s="2">
         <v>10.51</v>
       </c>
-      <c r="D7" s="2">
-        <v>143.0</v>
-      </c>
+      <c r="D7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="2">
@@ -199,9 +179,7 @@
       <c r="C8" s="2">
         <v>10.58</v>
       </c>
-      <c r="D8" s="2">
-        <v>143.0</v>
-      </c>
+      <c r="D8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="2">
@@ -213,9 +191,7 @@
       <c r="C9" s="2">
         <v>10.54</v>
       </c>
-      <c r="D9" s="2">
-        <v>143.0</v>
-      </c>
+      <c r="D9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="2">
@@ -227,9 +203,7 @@
       <c r="C10" s="2">
         <v>9.31</v>
       </c>
-      <c r="D10" s="2">
-        <v>135.0</v>
-      </c>
+      <c r="D10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="2">
@@ -241,9 +215,7 @@
       <c r="C11" s="2">
         <v>10.63</v>
       </c>
-      <c r="D11" s="2">
-        <v>143.0</v>
-      </c>
+      <c r="D11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" s="2">
@@ -255,9 +227,7 @@
       <c r="C12" s="2">
         <v>9.28</v>
       </c>
-      <c r="D12" s="2">
-        <v>135.0</v>
-      </c>
+      <c r="D12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="2">
@@ -269,9 +239,7 @@
       <c r="C13" s="2">
         <v>10.56</v>
       </c>
-      <c r="D13" s="2">
-        <v>143.0</v>
-      </c>
+      <c r="D13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" s="2">
@@ -283,9 +251,7 @@
       <c r="C14" s="2">
         <v>9.18</v>
       </c>
-      <c r="D14" s="2">
-        <v>135.0</v>
-      </c>
+      <c r="D14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" s="2">
@@ -297,9 +263,7 @@
       <c r="C15" s="2">
         <v>9.19</v>
       </c>
-      <c r="D15" s="2">
-        <v>135.0</v>
-      </c>
+      <c r="D15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" s="2">
@@ -311,9 +275,7 @@
       <c r="C16" s="2">
         <v>9.2</v>
       </c>
-      <c r="D16" s="2">
-        <v>135.0</v>
-      </c>
+      <c r="D16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" s="2">
@@ -325,9 +287,7 @@
       <c r="C17" s="2">
         <v>9.22</v>
       </c>
-      <c r="D17" s="2">
-        <v>135.0</v>
-      </c>
+      <c r="D17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" s="2">
@@ -339,9 +299,7 @@
       <c r="C18" s="2">
         <v>10.57</v>
       </c>
-      <c r="D18" s="2">
-        <v>143.0</v>
-      </c>
+      <c r="D18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" s="2">
@@ -353,9 +311,7 @@
       <c r="C19" s="2">
         <v>10.44</v>
       </c>
-      <c r="D19" s="2">
-        <v>143.0</v>
-      </c>
+      <c r="D19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" s="2">
@@ -367,9 +323,7 @@
       <c r="C20" s="2">
         <v>10.54</v>
       </c>
-      <c r="D20" s="2">
-        <v>143.0</v>
-      </c>
+      <c r="D20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" s="2">
@@ -381,9 +335,7 @@
       <c r="C21" s="2">
         <v>10.56</v>
       </c>
-      <c r="D21" s="2">
-        <v>143.0</v>
-      </c>
+      <c r="D21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" s="2">
@@ -395,9 +347,7 @@
       <c r="C22" s="2">
         <v>10.57</v>
       </c>
-      <c r="D22" s="2">
-        <v>143.0</v>
-      </c>
+      <c r="D22" s="2"/>
     </row>
     <row r="23">
       <c r="A23" s="2">
@@ -409,9 +359,7 @@
       <c r="C23" s="2">
         <v>9.23</v>
       </c>
-      <c r="D23" s="2">
-        <v>135.0</v>
-      </c>
+      <c r="D23" s="2"/>
     </row>
     <row r="24">
       <c r="A24" s="2">
@@ -423,9 +371,7 @@
       <c r="C24" s="2">
         <v>9.25</v>
       </c>
-      <c r="D24" s="2">
-        <v>135.0</v>
-      </c>
+      <c r="D24" s="2"/>
     </row>
     <row r="25">
       <c r="A25" s="2">
@@ -437,9 +383,7 @@
       <c r="C25" s="2">
         <v>9.27</v>
       </c>
-      <c r="D25" s="2">
-        <v>135.0</v>
-      </c>
+      <c r="D25" s="2"/>
     </row>
     <row r="26">
       <c r="A26" s="2">
@@ -451,9 +395,7 @@
       <c r="C26" s="2">
         <v>9.31</v>
       </c>
-      <c r="D26" s="2">
-        <v>135.0</v>
-      </c>
+      <c r="D26" s="2"/>
     </row>
     <row r="27">
       <c r="A27" s="2">
@@ -465,9 +407,7 @@
       <c r="C27" s="2">
         <v>9.96</v>
       </c>
-      <c r="D27" s="2">
-        <v>139.0</v>
-      </c>
+      <c r="D27" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>